<commit_message>
Bugs Fixed and Cooling Effect Done
</commit_message>
<xml_diff>
--- a/Result2.xlsx
+++ b/Result2.xlsx
@@ -830,25 +830,25 @@
         <v>0.2</v>
       </c>
       <c r="E10">
-        <v>8.550000000000001</v>
+        <v>8.380000000000001</v>
       </c>
       <c r="F10">
         <v>594</v>
       </c>
       <c r="G10">
-        <v>-77.22</v>
+        <v>468.62</v>
       </c>
       <c r="H10">
-        <v>-1.263800195015449</v>
+        <v>9.038038375901294</v>
       </c>
       <c r="I10">
-        <v>69.85645748820389</v>
+        <v>75.1961981462664</v>
       </c>
       <c r="J10">
         <v>1</v>
       </c>
       <c r="K10">
-        <v>-0.03</v>
+        <v>0.19</v>
       </c>
       <c r="L10" t="s">
         <v>13</v>
@@ -874,25 +874,25 @@
         <v>1</v>
       </c>
       <c r="E11">
-        <v>8.619999999999999</v>
+        <v>8.44</v>
       </c>
       <c r="F11">
         <v>602</v>
       </c>
       <c r="G11">
-        <v>-77.84999999999999</v>
+        <v>475.46</v>
       </c>
       <c r="H11">
-        <v>-0.4771398042572628</v>
+        <v>9.963588420820088</v>
       </c>
       <c r="I11">
-        <v>70.30362842435716</v>
+        <v>75.73501523426967</v>
       </c>
       <c r="J11">
         <v>1</v>
       </c>
       <c r="K11">
-        <v>-0.03</v>
+        <v>0.2</v>
       </c>
       <c r="L11" t="s">
         <v>13</v>
@@ -918,25 +918,25 @@
         <v>1.4</v>
       </c>
       <c r="E12">
-        <v>8.699999999999999</v>
+        <v>8.51</v>
       </c>
       <c r="F12">
         <v>614</v>
       </c>
       <c r="G12">
-        <v>-78.55</v>
+        <v>485.92</v>
       </c>
       <c r="H12">
-        <v>-0.09588297043063676</v>
+        <v>10.55336407969622</v>
       </c>
       <c r="I12">
-        <v>70.52162321400827</v>
+        <v>76.07276696851476</v>
       </c>
       <c r="J12">
         <v>1</v>
       </c>
       <c r="K12">
-        <v>-0.03</v>
+        <v>0.2</v>
       </c>
       <c r="L12" t="s">
         <v>13</v>
@@ -962,25 +962,25 @@
         <v>2</v>
       </c>
       <c r="E13">
-        <v>7.46</v>
+        <v>7.32</v>
       </c>
       <c r="F13">
         <v>522</v>
       </c>
       <c r="G13">
-        <v>-67.39</v>
+        <v>412.26</v>
       </c>
       <c r="H13">
-        <v>0.7355723598356576</v>
+        <v>9.793185203867267</v>
       </c>
       <c r="I13">
-        <v>70.98216910695191</v>
+        <v>75.70516509923618</v>
       </c>
       <c r="J13">
         <v>1</v>
       </c>
       <c r="K13">
-        <v>-0.03</v>
+        <v>0.17</v>
       </c>
       <c r="L13" t="s">
         <v>13</v>
@@ -1006,25 +1006,25 @@
         <v>2.5</v>
       </c>
       <c r="E14">
-        <v>4.67</v>
+        <v>4.62</v>
       </c>
       <c r="F14">
         <v>320</v>
       </c>
       <c r="G14">
-        <v>-42.25</v>
+        <v>251.4</v>
       </c>
       <c r="H14">
-        <v>1.746205523641038</v>
+        <v>7.304037140469404</v>
       </c>
       <c r="I14">
-        <v>71.5305090919137</v>
+        <v>74.42060444317758</v>
       </c>
       <c r="J14">
         <v>1</v>
       </c>
       <c r="K14">
-        <v>-0.02</v>
+        <v>0.11</v>
       </c>
       <c r="L14" t="s">
         <v>13</v>
@@ -1056,19 +1056,19 @@
         <v>57</v>
       </c>
       <c r="G15">
-        <v>-7.52</v>
+        <v>44.71</v>
       </c>
       <c r="H15">
-        <v>3.027231892662087</v>
+        <v>4.018826999725093</v>
       </c>
       <c r="I15">
-        <v>72.22680880327243</v>
+        <v>72.74050571763655</v>
       </c>
       <c r="J15">
         <v>1</v>
       </c>
       <c r="K15">
-        <v>-0</v>
+        <v>0.02</v>
       </c>
       <c r="L15" t="s">
         <v>13</v>
@@ -1795,25 +1795,25 @@
         <v>29.5</v>
       </c>
       <c r="E32">
-        <v>38.83</v>
+        <v>38.09999999999999</v>
       </c>
       <c r="F32">
         <v>2709</v>
       </c>
       <c r="G32">
-        <v>-350.78</v>
+        <v>2138.37</v>
       </c>
       <c r="H32">
-        <v>22.97218680643543</v>
+        <v>69.97104022047938</v>
       </c>
       <c r="I32">
-        <v>425.4211961287074</v>
+        <v>449.8702556091012</v>
       </c>
       <c r="J32">
         <v>6</v>
       </c>
       <c r="K32">
-        <v>-0.14</v>
+        <v>0.8900000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>